<commit_message>
Change to Readme, Initial commit of software
</commit_message>
<xml_diff>
--- a/Payment_records.xlsx
+++ b/Payment_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leowo\Dev\EPFL\Bachelor_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DCC49E-265F-48DA-9D29-862290984ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B33D07-0A9E-442F-8424-0AE5BD781495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7819C851-DC0A-4C3D-AF75-45B362737226}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="35">
   <si>
     <t>MDF 6mm</t>
   </si>
@@ -108,6 +108,39 @@
   </si>
   <si>
     <t>Other prices</t>
+  </si>
+  <si>
+    <t>Screws M3x20-22</t>
+  </si>
+  <si>
+    <t>Screws M4x12</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Price/Unit</t>
+  </si>
+  <si>
+    <t>Consumable Price</t>
+  </si>
+  <si>
+    <t>PETG Blanc</t>
+  </si>
+  <si>
+    <t>PETG Noir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPOT </t>
+  </si>
+  <si>
+    <t>Screws &amp; Nuts</t>
+  </si>
+  <si>
+    <t>Scres, Nuts &amp; Aluminium</t>
+  </si>
+  <si>
+    <t>Screws</t>
   </si>
 </sst>
 </file>
@@ -460,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6298D710-86AB-4E1C-AE3F-7EBA856A63EA}">
-  <dimension ref="B2:T158"/>
+  <dimension ref="B2:U158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +507,7 @@
     <col min="13" max="13" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -517,8 +550,17 @@
       <c r="O2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>44872</v>
       </c>
@@ -557,8 +599,12 @@
       <c r="O3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R3">
+        <f>P3*Q3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>44873</v>
       </c>
@@ -572,28 +618,32 @@
         <v>295</v>
       </c>
       <c r="F4">
-        <f>(D4/1000) * (E4/1000)</f>
+        <f t="shared" ref="F4:F10" si="0">(D4/1000) * (E4/1000)</f>
         <v>0.16225000000000001</v>
       </c>
       <c r="G4">
         <v>13</v>
       </c>
       <c r="H4">
-        <f xml:space="preserve"> F4*G4</f>
+        <f t="shared" ref="H4:H10" si="1" xml:space="preserve"> F4*G4</f>
         <v>2.1092500000000003</v>
       </c>
       <c r="K4" t="s">
         <v>14</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N67" si="0">L4 * M4</f>
+        <f t="shared" ref="N4:N67" si="2">L4 * M4</f>
         <v>0</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R4">
+        <f t="shared" ref="R4:R67" si="3">P4*Q4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>44873</v>
       </c>
@@ -607,14 +657,14 @@
         <v>160</v>
       </c>
       <c r="F5">
-        <f>(D5/1000) * (E5/1000)</f>
+        <f t="shared" si="0"/>
         <v>8.1280000000000005E-2</v>
       </c>
       <c r="G5">
         <v>13</v>
       </c>
       <c r="H5">
-        <f xml:space="preserve"> F5*G5</f>
+        <f t="shared" si="1"/>
         <v>1.05664</v>
       </c>
       <c r="I5">
@@ -628,14 +678,18 @@
         <v>14</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>44874</v>
       </c>
@@ -649,28 +703,32 @@
         <v>265</v>
       </c>
       <c r="F6">
-        <f>(D6/1000) * (E6/1000)</f>
+        <f t="shared" si="0"/>
         <v>0.14177500000000001</v>
       </c>
       <c r="G6">
         <v>13</v>
       </c>
       <c r="H6">
-        <f xml:space="preserve"> F6*G6</f>
+        <f t="shared" si="1"/>
         <v>1.8430750000000002</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>44874</v>
       </c>
@@ -684,28 +742,32 @@
         <v>219</v>
       </c>
       <c r="F7">
-        <f>(D7/1000) * (E7/1000)</f>
+        <f t="shared" si="0"/>
         <v>6.0225000000000008E-2</v>
       </c>
       <c r="G7">
         <v>13</v>
       </c>
       <c r="H7">
-        <f xml:space="preserve"> F7*G7</f>
+        <f t="shared" si="1"/>
         <v>0.78292500000000009</v>
       </c>
       <c r="K7" t="s">
         <v>14</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>44874</v>
       </c>
@@ -719,28 +781,32 @@
         <v>182</v>
       </c>
       <c r="F8">
-        <f>(D8/1000) * (E8/1000)</f>
+        <f t="shared" si="0"/>
         <v>4.3679999999999997E-2</v>
       </c>
       <c r="G8">
         <v>13</v>
       </c>
       <c r="H8">
-        <f xml:space="preserve"> F8*G8</f>
+        <f t="shared" si="1"/>
         <v>0.5678399999999999</v>
       </c>
       <c r="K8" t="s">
         <v>14</v>
       </c>
       <c r="N8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>44874</v>
       </c>
@@ -754,28 +820,32 @@
         <v>250</v>
       </c>
       <c r="F9">
-        <f>(D9/1000) * (E9/1000)</f>
+        <f t="shared" si="0"/>
         <v>0.115</v>
       </c>
       <c r="G9">
         <v>13</v>
       </c>
       <c r="H9">
-        <f xml:space="preserve"> F9*G9</f>
+        <f t="shared" si="1"/>
         <v>1.4950000000000001</v>
       </c>
       <c r="K9" t="s">
         <v>14</v>
       </c>
       <c r="N9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>44874</v>
       </c>
@@ -789,14 +859,14 @@
         <v>201</v>
       </c>
       <c r="F10">
-        <f>(D10/1000) * (E10/1000)</f>
+        <f t="shared" si="0"/>
         <v>4.9446000000000004E-2</v>
       </c>
       <c r="G10">
         <v>13</v>
       </c>
       <c r="H10">
-        <f xml:space="preserve"> F10*G10</f>
+        <f t="shared" si="1"/>
         <v>0.64279800000000009</v>
       </c>
       <c r="I10">
@@ -810,24 +880,28 @@
         <v>14</v>
       </c>
       <c r="N10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
         <v>16</v>
       </c>
-      <c r="S10">
-        <f>SUM(H3:H128) + SUM(N3:N128)+ SUM(O3:O128)</f>
-        <v>15.192025952000002</v>
-      </c>
-      <c r="T10" t="s">
+      <c r="T10">
+        <f>SUM(H3:H128) + SUM(N3:N128)+ SUM(O3:O128)+ SUM(R3:R128)</f>
+        <v>19.843520951999999</v>
+      </c>
+      <c r="U10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>44890</v>
       </c>
@@ -860,14 +934,18 @@
         <v>15</v>
       </c>
       <c r="N11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>44893</v>
       </c>
@@ -881,14 +959,14 @@
         <v>159.03</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F4:F67" si="1">(D12/1000) * (E12/1000)</f>
+        <f t="shared" ref="F12:F67" si="4">(D12/1000) * (E12/1000)</f>
         <v>8.7466499999999999E-3</v>
       </c>
       <c r="G12">
         <v>10.88</v>
       </c>
       <c r="H12">
-        <f t="shared" ref="H4:H67" si="2" xml:space="preserve"> F12*G12</f>
+        <f t="shared" ref="H12:H67" si="5" xml:space="preserve"> F12*G12</f>
         <v>9.5163552000000012E-2</v>
       </c>
       <c r="J12" t="s">
@@ -898,14 +976,18 @@
         <v>15</v>
       </c>
       <c r="N12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>44893</v>
       </c>
@@ -913,11 +995,11 @@
         <v>20</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J13" t="s">
@@ -930,14 +1012,18 @@
         <v>33.840000000000003</v>
       </c>
       <c r="N13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>44893</v>
       </c>
@@ -945,11 +1031,11 @@
         <v>20</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J14" t="s">
@@ -962,14 +1048,18 @@
         <v>22</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>44893</v>
       </c>
@@ -983,14 +1073,14 @@
         <v>166</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>9.130000000000001E-3</v>
       </c>
       <c r="G15">
         <v>10.88</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>9.9334400000000017E-2</v>
       </c>
       <c r="J15" t="s">
@@ -1000,2441 +1090,3270 @@
         <v>15</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="R15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>44893</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" t="s">
+        <v>15</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="P16">
+        <v>16</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>44893</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" t="s">
+        <v>15</v>
       </c>
       <c r="N17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="P17">
+        <v>12</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>44894</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>150</v>
+      </c>
+      <c r="E18">
+        <v>205</v>
+      </c>
       <c r="F18">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>3.0749999999999996E-2</v>
+      </c>
+      <c r="G18">
+        <v>10.88</v>
       </c>
       <c r="H18">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.33455999999999997</v>
+      </c>
+      <c r="J18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" t="s">
+        <v>15</v>
       </c>
       <c r="N18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>44894</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
       <c r="F19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" t="s">
+        <v>15</v>
+      </c>
+      <c r="L19">
+        <v>23</v>
       </c>
       <c r="N19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>44894</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
       <c r="F20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H20">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20">
+        <v>40</v>
       </c>
       <c r="N20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <v>44894</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
       <c r="F21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21">
+        <v>34</v>
       </c>
       <c r="N21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <v>44895</v>
+      </c>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
       <c r="F22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22">
+        <v>29</v>
       </c>
       <c r="N22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>44900</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23">
+        <v>45</v>
       </c>
       <c r="N23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>44900</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
       <c r="F24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" t="s">
+        <v>15</v>
+      </c>
+      <c r="L24">
+        <v>37</v>
       </c>
       <c r="N24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>44900</v>
+      </c>
+      <c r="C25" t="s">
+        <v>29</v>
+      </c>
       <c r="F25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K25" t="s">
+        <v>31</v>
+      </c>
+      <c r="L25">
+        <v>23</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
+        <v>44900</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>556</v>
+      </c>
+      <c r="E26">
+        <v>220</v>
+      </c>
       <c r="F26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>0.12232000000000001</v>
+      </c>
+      <c r="G26">
+        <v>13</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>1.5901600000000002</v>
+      </c>
+      <c r="J26" t="s">
+        <v>11</v>
+      </c>
+      <c r="K26" t="s">
+        <v>15</v>
       </c>
       <c r="N26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>44900</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>85</v>
+      </c>
+      <c r="E27">
+        <v>255</v>
+      </c>
       <c r="F27">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2.1675000000000003E-2</v>
+      </c>
+      <c r="G27">
+        <v>13</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.28177500000000005</v>
       </c>
       <c r="N27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B28" s="1">
+        <v>44901</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
       <c r="F28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
+      <c r="M28">
+        <f>20/1000</f>
+        <v>0.02</v>
       </c>
       <c r="N28">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="O28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B29" s="1">
+        <v>44901</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
+      </c>
       <c r="F29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>1.5</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
+        <v>44902</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
       <c r="F30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>0.45</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
+        <v>44902</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
       <c r="F31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="P31">
+        <v>3.4</v>
+      </c>
+      <c r="Q31">
+        <v>0.05</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="3"/>
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B32" s="1">
+        <v>44902</v>
+      </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
       <c r="F32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="P32">
+        <v>4.5</v>
+      </c>
+      <c r="Q32">
+        <v>0.05</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="3"/>
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R34">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R40">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R41">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R42">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R43">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R44">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R45">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R46">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R47">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R48">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R49">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R51">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R52">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R53">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R54">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R55">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R56">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R57">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R58">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R59">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R60">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R61">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R62">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R63">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R65">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R66">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F67">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R67">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F68">
-        <f t="shared" ref="F68:F131" si="3">(D68/1000) * (E68/1000)</f>
+        <f t="shared" ref="F68:F131" si="6">(D68/1000) * (E68/1000)</f>
         <v>0</v>
       </c>
       <c r="H68">
-        <f t="shared" ref="H68:H131" si="4" xml:space="preserve"> F68*G68</f>
+        <f t="shared" ref="H68:H131" si="7" xml:space="preserve"> F68*G68</f>
         <v>0</v>
       </c>
       <c r="N68">
-        <f t="shared" ref="N68:N131" si="5">L68 * M68</f>
+        <f t="shared" ref="N68:N131" si="8">L68 * M68</f>
         <v>0</v>
       </c>
       <c r="O68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R68">
+        <f t="shared" ref="R68:R131" si="9">P68*Q68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R69">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R70">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R71">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R72">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R73">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R74">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R75">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R76">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R77">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R78">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R79">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R80">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R81">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R82">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R83">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R84">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R85">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R86">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R87">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R88">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R89">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R90">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R91">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R92">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R93">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R94">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R95">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R96">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R97">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R98">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R99">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R100">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R101">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R102">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F103">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R103">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F104">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R104">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F105">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R105">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R106">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F107">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R107">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F108">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R108">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F109">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R109">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F110">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R110">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F111">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R111">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F112">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R112">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F113">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R113">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F114">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H114">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R114">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F115">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H115">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R115">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F116">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H116">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R116">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F117">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H117">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R117">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F118">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H118">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R118">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F119">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H119">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R119">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F120">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R120">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F121">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H121">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R121">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F122">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H122">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R122">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F123">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R123">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F124">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R124">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F125">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H125">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R125">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F126">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H126">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O126">
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R126">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F127">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O127">
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R127">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F128">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O128">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R128">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F129">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H129">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N129">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O129">
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R129">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F130">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H130">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N130">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O130">
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R130">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F131">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H131">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N131">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O131">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R131">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F132">
-        <f t="shared" ref="F132:F158" si="6">(D132/1000) * (E132/1000)</f>
+        <f t="shared" ref="F132:F158" si="10">(D132/1000) * (E132/1000)</f>
         <v>0</v>
       </c>
       <c r="H132">
-        <f t="shared" ref="H132:H158" si="7" xml:space="preserve"> F132*G132</f>
+        <f t="shared" ref="H132:H158" si="11" xml:space="preserve"> F132*G132</f>
         <v>0</v>
       </c>
       <c r="N132">
-        <f t="shared" ref="N132:N158" si="8">L132 * M132</f>
+        <f t="shared" ref="N132:N158" si="12">L132 * M132</f>
         <v>0</v>
       </c>
       <c r="O132">
         <v>0</v>
       </c>
-    </row>
-    <row r="133" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R132">
+        <f t="shared" ref="R132:R158" si="13">P132*Q132</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F133">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H133">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N133">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O133">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R133">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F134">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H134">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N134">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O134">
         <v>0</v>
       </c>
-    </row>
-    <row r="135" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R134">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F135">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H135">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N135">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O135">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R135">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F136">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H136">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N136">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O136">
         <v>0</v>
       </c>
-    </row>
-    <row r="137" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R136">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F137">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H137">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N137">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O137">
         <v>0</v>
       </c>
-    </row>
-    <row r="138" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R137">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F138">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H138">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N138">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O138">
         <v>0</v>
       </c>
-    </row>
-    <row r="139" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R138">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F139">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H139">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N139">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O139">
         <v>0</v>
       </c>
-    </row>
-    <row r="140" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R139">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F140">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H140">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N140">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O140">
         <v>0</v>
       </c>
-    </row>
-    <row r="141" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R140">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F141">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H141">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N141">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O141">
         <v>0</v>
       </c>
-    </row>
-    <row r="142" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R141">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F142">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H142">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N142">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O142">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R142">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F143">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H143">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N143">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O143">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R143">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F144">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H144">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N144">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O144">
         <v>0</v>
       </c>
-    </row>
-    <row r="145" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R144">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F145">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H145">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N145">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O145">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R145">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F146">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H146">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N146">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R146">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F147">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H147">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N147">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R147">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F148">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H148">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N148">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O148">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R148">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F149">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H149">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N149">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O149">
         <v>0</v>
       </c>
-    </row>
-    <row r="150" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R149">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F150">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H150">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N150">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O150">
         <v>0</v>
       </c>
-    </row>
-    <row r="151" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R150">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F151">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H151">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N151">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O151">
         <v>0</v>
       </c>
-    </row>
-    <row r="152" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R151">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F152">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H152">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N152">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O152">
         <v>0</v>
       </c>
-    </row>
-    <row r="153" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R152">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F153">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H153">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N153">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R153">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F154">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H154">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N154">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O154">
         <v>0</v>
       </c>
-    </row>
-    <row r="155" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R154">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F155">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H155">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N155">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O155">
         <v>0</v>
       </c>
-    </row>
-    <row r="156" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R155">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F156">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H156">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N156">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O156">
         <v>0</v>
       </c>
-    </row>
-    <row r="157" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R156">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F157">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H157">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N157">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O157">
         <v>0</v>
       </c>
-    </row>
-    <row r="158" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R157">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="6:18" x14ac:dyDescent="0.3">
       <c r="F158">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="H158">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N158">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O158">
+        <v>0</v>
+      </c>
+      <c r="R158">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add description for scholar papers
</commit_message>
<xml_diff>
--- a/Payment_records.xlsx
+++ b/Payment_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leowo\Dev\EPFL\Bachelor_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B33D07-0A9E-442F-8424-0AE5BD781495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70BAD4A-988C-4C44-BE02-E9EFE031E764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7819C851-DC0A-4C3D-AF75-45B362737226}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="36">
   <si>
     <t>MDF 6mm</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Screws</t>
+  </si>
+  <si>
+    <t>PETG</t>
   </si>
 </sst>
 </file>
@@ -495,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6298D710-86AB-4E1C-AE3F-7EBA856A63EA}">
   <dimension ref="B2:U158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1711,7 +1714,13 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="33" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
+        <v>44902</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
       <c r="F33">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1720,6 +1729,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L33">
+        <v>131</v>
+      </c>
       <c r="N33">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -1732,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F34">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1753,7 +1765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F35">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1774,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F36">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1795,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F37">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1816,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F38">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1837,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F39">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1858,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F40">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1879,7 +1891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F41">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1900,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F42">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1921,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F43">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1942,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F44">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1963,7 +1975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F45">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1984,7 +1996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F46">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2005,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F47">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2026,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
       <c r="F48">
         <f t="shared" si="4"/>
         <v>0</v>

</xml_diff>

<commit_message>
Update README.md + Resources
</commit_message>
<xml_diff>
--- a/Payment_records.xlsx
+++ b/Payment_records.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leowo\Dev\EPFL\Bachelor_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{727F7907-7E45-4781-BF61-682757BF9080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA6BAB6-85DF-4E30-B2AF-9F33B29E91FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7819C851-DC0A-4C3D-AF75-45B362737226}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="38">
   <si>
     <t>MDF 6mm</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Screws and nuts</t>
+  </si>
+  <si>
+    <t>Screws and Nuts</t>
   </si>
 </sst>
 </file>
@@ -501,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6298D710-86AB-4E1C-AE3F-7EBA856A63EA}">
   <dimension ref="B2:U158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,7 +904,7 @@
       </c>
       <c r="T10">
         <f>SUM(H3:H128) + SUM(N3:N128)+ SUM(O3:O128)+ SUM(R3:R128)</f>
-        <v>26.881384952000001</v>
+        <v>53.543384952000004</v>
       </c>
       <c r="U10" t="s">
         <v>17</v>
@@ -1017,9 +1020,12 @@
       <c r="L13">
         <v>33.840000000000003</v>
       </c>
+      <c r="M13">
+        <v>0.05</v>
+      </c>
       <c r="N13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.6920000000000002</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1053,9 +1059,12 @@
       <c r="L14">
         <v>22</v>
       </c>
+      <c r="M14">
+        <v>0.05</v>
+      </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -1245,9 +1254,12 @@
       <c r="L19">
         <v>23</v>
       </c>
+      <c r="M19">
+        <v>0.05</v>
+      </c>
       <c r="N19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1500000000000001</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1281,9 +1293,12 @@
       <c r="L20">
         <v>40</v>
       </c>
+      <c r="M20">
+        <v>0.05</v>
+      </c>
       <c r="N20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1317,9 +1332,12 @@
       <c r="L21">
         <v>34</v>
       </c>
+      <c r="M21">
+        <v>0.05</v>
+      </c>
       <c r="N21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1353,9 +1371,12 @@
       <c r="L22">
         <v>29</v>
       </c>
+      <c r="M22">
+        <v>0.05</v>
+      </c>
       <c r="N22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.4500000000000002</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1389,9 +1410,12 @@
       <c r="L23">
         <v>45</v>
       </c>
+      <c r="M23">
+        <v>0.05</v>
+      </c>
       <c r="N23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1425,9 +1449,12 @@
       <c r="L24">
         <v>37</v>
       </c>
+      <c r="M24">
+        <v>0.05</v>
+      </c>
       <c r="N24">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.85</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1461,9 +1488,12 @@
       <c r="L25">
         <v>23</v>
       </c>
+      <c r="M25">
+        <v>0.05</v>
+      </c>
       <c r="N25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.1500000000000001</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1777,9 +1807,12 @@
       <c r="L33">
         <v>131</v>
       </c>
+      <c r="M33">
+        <v>0.05</v>
+      </c>
       <c r="N33">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5500000000000007</v>
       </c>
       <c r="O33">
         <v>0</v>
@@ -2006,6 +2039,12 @@
       </c>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B40" s="1">
+        <v>44938</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
       <c r="F40">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2021,12 +2060,24 @@
       <c r="O40">
         <v>0</v>
       </c>
+      <c r="P40">
+        <v>38</v>
+      </c>
+      <c r="Q40">
+        <v>0.05</v>
+      </c>
       <c r="R40">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.9000000000000001</v>
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B41" s="1">
+        <v>44938</v>
+      </c>
+      <c r="C41" t="s">
+        <v>35</v>
+      </c>
       <c r="F41">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2035,9 +2086,15 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L41">
+        <v>48</v>
+      </c>
+      <c r="M41">
+        <v>0.05</v>
+      </c>
       <c r="N41">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="O41">
         <v>0</v>
@@ -2048,6 +2105,12 @@
       </c>
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <v>44939</v>
+      </c>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
       <c r="F42">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2063,12 +2126,24 @@
       <c r="O42">
         <v>0</v>
       </c>
+      <c r="P42">
+        <v>12</v>
+      </c>
+      <c r="Q42">
+        <v>0.05</v>
+      </c>
       <c r="R42">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.60000000000000009</v>
       </c>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B43" s="1">
+        <v>44939</v>
+      </c>
+      <c r="C43" t="s">
+        <v>34</v>
+      </c>
       <c r="F43">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2084,12 +2159,24 @@
       <c r="O43">
         <v>0</v>
       </c>
+      <c r="P43">
+        <v>10</v>
+      </c>
+      <c r="Q43">
+        <v>0.05</v>
+      </c>
       <c r="R43">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B44" s="1">
+        <v>44939</v>
+      </c>
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
       <c r="F44">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2105,9 +2192,15 @@
       <c r="O44">
         <v>0</v>
       </c>
+      <c r="P44">
+        <v>7.4</v>
+      </c>
+      <c r="Q44">
+        <v>0.05</v>
+      </c>
       <c r="R44">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.37000000000000005</v>
       </c>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Commit last changes to the on the model and switch holders
</commit_message>
<xml_diff>
--- a/Payment_records.xlsx
+++ b/Payment_records.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leowo\Dev\EPFL\Bachelor_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D7CFB3-748B-4321-B472-2C8EA9196562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2430B89-B805-4BD3-AFAC-D14C7D60D925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7819C851-DC0A-4C3D-AF75-45B362737226}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7819C851-DC0A-4C3D-AF75-45B362737226}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="39">
   <si>
     <t>MDF 6mm</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Daily Subtotal</t>
-  </si>
-  <si>
-    <t>Payed</t>
   </si>
   <si>
     <t>Yes</t>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Payed (By me), need refund</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -514,22 +514,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6298D710-86AB-4E1C-AE3F-7EBA856A63EA}">
   <dimension ref="B2:U158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="2"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
-    <col min="13" max="13" width="9.77734375" customWidth="1"/>
-    <col min="14" max="15" width="8.88671875" style="2"/>
-    <col min="18" max="18" width="8.88671875" style="2"/>
+    <col min="4" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="2"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+    <col min="14" max="15" width="8.85546875" style="2"/>
+    <col min="18" max="18" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -549,40 +549,40 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" t="s">
-        <v>19</v>
-      </c>
       <c r="N2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>44872</v>
       </c>
@@ -609,10 +609,10 @@
         <v>0.5</v>
       </c>
       <c r="J3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N3" s="2">
         <f>L3 * M3</f>
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>44873</v>
       </c>
@@ -651,10 +651,10 @@
         <v>2.1092500000000003</v>
       </c>
       <c r="J4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" ref="N4:N67" si="2">L4 * M4</f>
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>44873</v>
       </c>
@@ -697,10 +697,10 @@
         <v>3.1658900000000001</v>
       </c>
       <c r="J5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N5" s="2">
         <f t="shared" si="2"/>
@@ -714,7 +714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>44874</v>
       </c>
@@ -739,10 +739,10 @@
         <v>1.8430750000000002</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="2"/>
@@ -756,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>44874</v>
       </c>
@@ -781,10 +781,10 @@
         <v>0.78292500000000009</v>
       </c>
       <c r="J7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" si="2"/>
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>44874</v>
       </c>
@@ -823,10 +823,10 @@
         <v>0.5678399999999999</v>
       </c>
       <c r="J8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N8" s="2">
         <f t="shared" si="2"/>
@@ -840,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>44874</v>
       </c>
@@ -865,10 +865,10 @@
         <v>1.4950000000000001</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N9" s="2">
         <f t="shared" si="2"/>
@@ -882,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>44874</v>
       </c>
@@ -911,10 +911,10 @@
         <v>5.3316380000000008</v>
       </c>
       <c r="J10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N10" s="2">
         <f t="shared" si="2"/>
@@ -928,22 +928,22 @@
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T10">
         <f>SUM(H3:H128) + SUM(N3:N128)+ SUM(O3:O128)+ SUM(R3:R128)</f>
         <v>64.078384952000008</v>
       </c>
       <c r="U10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>44890</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -965,10 +965,10 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N11" s="2">
         <f t="shared" si="2"/>
@@ -982,7 +982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>44893</v>
       </c>
@@ -1007,10 +1007,10 @@
         <v>9.5163552000000012E-2</v>
       </c>
       <c r="J12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N12" s="2">
         <f t="shared" si="2"/>
@@ -1024,12 +1024,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>44893</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <f t="shared" si="4"/>
@@ -1040,10 +1040,10 @@
         <v>0</v>
       </c>
       <c r="J13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L13">
         <v>33.840000000000003</v>
@@ -1063,12 +1063,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>44893</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14">
         <f t="shared" si="4"/>
@@ -1079,10 +1079,10 @@
         <v>0</v>
       </c>
       <c r="J14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L14">
         <v>22</v>
@@ -1102,7 +1102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>44893</v>
       </c>
@@ -1127,10 +1127,10 @@
         <v>9.9334400000000017E-2</v>
       </c>
       <c r="J15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="2"/>
@@ -1144,12 +1144,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>44893</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
@@ -1160,10 +1160,10 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="2"/>
@@ -1180,12 +1180,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>44893</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F17">
         <f t="shared" si="4"/>
@@ -1196,10 +1196,10 @@
         <v>0</v>
       </c>
       <c r="J17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="2"/>
@@ -1216,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>44894</v>
       </c>
@@ -1241,10 +1241,10 @@
         <v>0.33455999999999997</v>
       </c>
       <c r="J18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="2"/>
@@ -1258,12 +1258,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>44894</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19">
         <f t="shared" si="4"/>
@@ -1274,10 +1274,10 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L19">
         <v>23</v>
@@ -1297,12 +1297,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>44894</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20">
         <f t="shared" si="4"/>
@@ -1313,10 +1313,10 @@
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L20">
         <v>40</v>
@@ -1336,12 +1336,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>44894</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21">
         <f t="shared" si="4"/>
@@ -1352,10 +1352,10 @@
         <v>0</v>
       </c>
       <c r="J21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L21">
         <v>34</v>
@@ -1375,12 +1375,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>44895</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F22">
         <f t="shared" si="4"/>
@@ -1391,10 +1391,10 @@
         <v>0</v>
       </c>
       <c r="J22" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L22">
         <v>29</v>
@@ -1414,12 +1414,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>44900</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23">
         <f t="shared" si="4"/>
@@ -1430,10 +1430,10 @@
         <v>0</v>
       </c>
       <c r="J23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L23">
         <v>45</v>
@@ -1453,12 +1453,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>44900</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F24">
         <f t="shared" si="4"/>
@@ -1469,10 +1469,10 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L24">
         <v>37</v>
@@ -1492,12 +1492,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>44900</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25">
         <f t="shared" si="4"/>
@@ -1508,10 +1508,10 @@
         <v>0</v>
       </c>
       <c r="J25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L25">
         <v>23</v>
@@ -1531,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>44900</v>
       </c>
@@ -1556,10 +1556,10 @@
         <v>1.5901600000000002</v>
       </c>
       <c r="J26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N26" s="2">
         <f t="shared" si="2"/>
@@ -1573,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>44900</v>
       </c>
@@ -1598,10 +1598,10 @@
         <v>0.28177500000000005</v>
       </c>
       <c r="J27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N27" s="2">
         <f t="shared" si="2"/>
@@ -1615,12 +1615,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>44901</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F28">
         <f t="shared" si="4"/>
@@ -1631,10 +1631,10 @@
         <v>0</v>
       </c>
       <c r="J28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L28">
         <v>5</v>
@@ -1655,12 +1655,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>44901</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F29">
         <f t="shared" si="4"/>
@@ -1671,10 +1671,10 @@
         <v>0</v>
       </c>
       <c r="J29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N29" s="2">
         <f t="shared" si="2"/>
@@ -1694,12 +1694,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>44902</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F30">
         <f t="shared" si="4"/>
@@ -1710,10 +1710,10 @@
         <v>0</v>
       </c>
       <c r="J30" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N30" s="2">
         <f t="shared" si="2"/>
@@ -1733,12 +1733,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>44902</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31">
         <f t="shared" si="4"/>
@@ -1749,10 +1749,10 @@
         <v>0</v>
       </c>
       <c r="J31" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N31" s="2">
         <f t="shared" si="2"/>
@@ -1772,12 +1772,12 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>44902</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F32">
         <f t="shared" si="4"/>
@@ -1788,10 +1788,10 @@
         <v>0</v>
       </c>
       <c r="J32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N32" s="2">
         <f t="shared" si="2"/>
@@ -1811,12 +1811,12 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>44902</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33">
         <f t="shared" si="4"/>
@@ -1827,10 +1827,10 @@
         <v>0</v>
       </c>
       <c r="J33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L33">
         <v>131</v>
@@ -1850,7 +1850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>44907</v>
       </c>
@@ -1875,10 +1875,10 @@
         <v>1.9737899999999999</v>
       </c>
       <c r="J34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N34" s="2">
         <f t="shared" si="2"/>
@@ -1892,12 +1892,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>44907</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F35">
         <f t="shared" si="4"/>
@@ -1908,10 +1908,10 @@
         <v>0</v>
       </c>
       <c r="J35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N35" s="2">
         <f t="shared" si="2"/>
@@ -1931,12 +1931,12 @@
         <v>0.78500000000000003</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>44908</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F36">
         <f t="shared" si="4"/>
@@ -1947,10 +1947,10 @@
         <v>0</v>
       </c>
       <c r="J36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N36" s="2">
         <f t="shared" si="2"/>
@@ -1970,7 +1970,7 @@
         <v>0.37000000000000005</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>44908</v>
       </c>
@@ -1995,10 +1995,10 @@
         <v>1.726842</v>
       </c>
       <c r="J37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N37" s="2">
         <f t="shared" si="2"/>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>44908</v>
       </c>
@@ -2037,10 +2037,10 @@
         <v>0.2392</v>
       </c>
       <c r="J38" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N38" s="2">
         <f t="shared" si="2"/>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>44909</v>
       </c>
@@ -2079,10 +2079,10 @@
         <v>1.9430319999999999</v>
       </c>
       <c r="J39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N39" s="2">
         <f t="shared" si="2"/>
@@ -2096,12 +2096,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>44938</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F40">
         <f t="shared" si="4"/>
@@ -2112,10 +2112,10 @@
         <v>0</v>
       </c>
       <c r="J40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N40" s="2">
         <f t="shared" si="2"/>
@@ -2135,12 +2135,12 @@
         <v>1.9000000000000001</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>44938</v>
       </c>
       <c r="C41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F41">
         <f t="shared" si="4"/>
@@ -2151,10 +2151,10 @@
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L41">
         <v>48</v>
@@ -2174,12 +2174,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>44939</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F42">
         <f t="shared" si="4"/>
@@ -2190,10 +2190,10 @@
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N42" s="2">
         <f t="shared" si="2"/>
@@ -2213,12 +2213,12 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>44939</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F43">
         <f t="shared" si="4"/>
@@ -2229,10 +2229,10 @@
         <v>0</v>
       </c>
       <c r="J43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N43" s="2">
         <f t="shared" si="2"/>
@@ -2252,12 +2252,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <v>44939</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F44">
         <f t="shared" si="4"/>
@@ -2268,10 +2268,10 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N44" s="2">
         <f t="shared" si="2"/>
@@ -2291,7 +2291,7 @@
         <v>0.37000000000000005</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
         <v>44942</v>
       </c>
@@ -2305,10 +2305,10 @@
         <v>1.7</v>
       </c>
       <c r="J45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N45" s="2">
         <f t="shared" si="2"/>
@@ -2322,12 +2322,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
         <v>44942</v>
       </c>
       <c r="C46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F46">
         <f t="shared" si="4"/>
@@ -2338,10 +2338,10 @@
         <v>0</v>
       </c>
       <c r="J46" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L46">
         <v>83</v>
@@ -2361,12 +2361,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <v>44942</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F47">
         <f t="shared" si="4"/>
@@ -2377,10 +2377,10 @@
         <v>0</v>
       </c>
       <c r="J47" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="N47" s="2">
         <f t="shared" si="2"/>
@@ -2400,12 +2400,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>44943</v>
       </c>
       <c r="C48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F48">
         <f t="shared" si="4"/>
@@ -2416,10 +2416,10 @@
         <v>0</v>
       </c>
       <c r="J48" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L48">
         <v>87</v>
@@ -2439,12 +2439,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>44943</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F49">
         <f t="shared" si="4"/>
@@ -2453,6 +2453,12 @@
       <c r="H49" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
+      </c>
+      <c r="J49" t="s">
+        <v>10</v>
+      </c>
+      <c r="K49" t="s">
+        <v>14</v>
       </c>
       <c r="N49" s="2">
         <f t="shared" si="2"/>
@@ -2472,7 +2478,7 @@
         <v>0.28500000000000003</v>
       </c>
     </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F50">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2493,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F51">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2514,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F52">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2535,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F53">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2556,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F54">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2577,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F55">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2598,7 +2604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F56">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2619,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F57">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2640,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F58">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2661,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F59">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2682,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F60">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2703,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F61">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2724,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F62">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2745,7 +2751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F63">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2766,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.25">
       <c r="F64">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2787,7 +2793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F65">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2808,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F66">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2829,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F67">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2850,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F68">
         <f t="shared" ref="F68:F131" si="6">(D68/1000) * (E68/1000)</f>
         <v>0</v>
@@ -2871,7 +2877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F69">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2892,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F70">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2913,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F71">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2934,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F72">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2955,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F73">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2976,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F74">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2997,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F75">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3018,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F76">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3039,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F77">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3060,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F78">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3081,7 +3087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F79">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3102,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F80">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3123,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F81">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3144,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F82">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3165,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F83">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3186,7 +3192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F84">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3207,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="85" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F85">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3228,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="86" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F86">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3249,7 +3255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="87" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F87">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3270,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="88" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F88">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3291,7 +3297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="89" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F89">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3312,7 +3318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="90" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F90">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3333,7 +3339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="91" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F91">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3354,7 +3360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="92" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F92">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3375,7 +3381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="93" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F93">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3396,7 +3402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="94" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F94">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3417,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="95" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F95">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3438,7 +3444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="96" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F96">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3459,7 +3465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="97" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F97">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3480,7 +3486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="98" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F98">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3501,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="99" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F99">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3522,7 +3528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="100" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F100">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3543,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="101" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F101">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3564,7 +3570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="102" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F102">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3585,7 +3591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="103" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F103">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3606,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="104" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F104">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3627,7 +3633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="105" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F105">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3648,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="106" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F106">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3669,7 +3675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="107" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F107">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3690,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="108" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F108">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3711,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="109" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F109">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3732,7 +3738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="110" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F110">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3753,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="111" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F111">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3774,7 +3780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="112" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F112">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3795,7 +3801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="113" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F113">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3816,7 +3822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="114" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F114">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3837,7 +3843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="115" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F115">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3858,7 +3864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="116" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F116">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3879,7 +3885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="117" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F117">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3900,7 +3906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="118" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F118">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3921,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="119" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F119">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3942,7 +3948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="120" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F120">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3963,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="121" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F121">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -3984,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="122" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F122">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4005,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="123" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F123">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4026,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="124" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F124">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4047,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="125" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F125">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4068,7 +4074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="126" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F126">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4089,7 +4095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="127" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F127">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4110,7 +4116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="128" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F128">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4131,7 +4137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="129" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F129">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4152,7 +4158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="130" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F130">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4173,7 +4179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="131" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F131">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4194,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="132" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F132">
         <f t="shared" ref="F132:F158" si="10">(D132/1000) * (E132/1000)</f>
         <v>0</v>
@@ -4215,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="133" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F133">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4236,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="134" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F134">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4257,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="135" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F135">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4278,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="136" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F136">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4299,7 +4305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="137" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F137">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4320,7 +4326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="138" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F138">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4341,7 +4347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="139" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F139">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4362,7 +4368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="140" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F140">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4383,7 +4389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="141" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F141">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4404,7 +4410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="142" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F142">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4425,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="143" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F143">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4446,7 +4452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="6:18" x14ac:dyDescent="0.3">
+    <row r="144" spans="6:18" x14ac:dyDescent="0.25">
       <c r="F144">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4467,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="145" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F145">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4488,7 +4494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="146" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F146">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4509,7 +4515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="147" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F147">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4530,7 +4536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="148" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F148">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4551,7 +4557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="149" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F149">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4572,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="150" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F150">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4593,7 +4599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="151" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F151">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4614,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="152" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F152">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4635,7 +4641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="153" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F153">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4656,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="154" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F154">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4677,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="155" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F155">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4698,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="156" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F156">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4719,7 +4725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="157" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F157">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4740,7 +4746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="6:21" x14ac:dyDescent="0.3">
+    <row r="158" spans="6:21" x14ac:dyDescent="0.25">
       <c r="F158">
         <f t="shared" si="10"/>
         <v>0</v>
@@ -4761,7 +4767,7 @@
         <v>0</v>
       </c>
       <c r="U158" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>